<commit_message>
[TMS][Update] Update template file for import training effect
</commit_message>
<xml_diff>
--- a/public/files/import_mark.xlsx
+++ b/public/files/import_mark.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA2542D-0235-48F0-A965-09499664644F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2F6AD2-5A1F-4A9C-A64F-CD6D932192B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>bichtuyen@easia-travel.com</t>
   </si>
@@ -83,22 +83,21 @@
   </si>
   <si>
     <t>com6</t>
+  </si>
+  <si>
+    <t>Competency code</t>
+  </si>
+  <si>
+    <t>Competency mark</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -115,14 +114,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,34 +157,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,7 +456,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,323 +467,327 @@
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
         <v>10</v>
       </c>
-      <c r="F3" s="4">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4">
-        <v>9</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="F3" s="2">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
         <v>10</v>
       </c>
-      <c r="F4" s="3">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="F4" s="4">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="B5" s="4">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3">
-        <v>7</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="F5" s="4">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="F6" s="3">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3">
-        <v>8</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="F6" s="4">
+        <v>7</v>
+      </c>
+      <c r="G6" s="4">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="B7" s="4">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="F7" s="3">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3">
-        <v>9</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="F7" s="4">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4">
+        <v>9</v>
+      </c>
+      <c r="H7" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3">
-        <v>8</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="C8" s="4">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>8</v>
+      </c>
+      <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="4">
-        <v>7</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8" s="2">
+        <v>7</v>
+      </c>
+      <c r="H8" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="3">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4">
-        <v>7</v>
-      </c>
-      <c r="F9" s="3">
-        <v>6</v>
-      </c>
-      <c r="G9" s="4">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="C9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
         <v>5</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>5</v>
       </c>
-      <c r="D10" s="3">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4">
-        <v>8</v>
-      </c>
-      <c r="F10" s="4">
-        <v>7</v>
-      </c>
-      <c r="G10" s="3">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="D10" s="4">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4">
-        <v>8</v>
-      </c>
-      <c r="G11" s="3">
-        <v>6</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="4">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4">
-        <v>7</v>
-      </c>
-      <c r="F12" s="4">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3">
-        <v>7</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
+        <v>8</v>
+      </c>
+      <c r="G12" s="4">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3">
-        <v>8</v>
-      </c>
-      <c r="E13" s="4">
-        <v>8</v>
-      </c>
-      <c r="F13" s="4">
-        <v>7</v>
-      </c>
-      <c r="G13" s="3">
-        <v>8</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7</v>
+      </c>
+      <c r="G13" s="4">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2">
         <v>9</v>
       </c>
     </row>

</xml_diff>